<commit_message>
Add some null tests for Range Intersect method
</commit_message>
<xml_diff>
--- a/Test Cases.xlsx
+++ b/Test Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohammadreza/UofC/SENG 637/seng637-a2-mreza-kiani/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2386894D-2E0A-794B-BED6-08EFF08D89B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E474316-CB1F-7C47-A01E-FA93C57B063B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="166">
   <si>
     <t>Range</t>
   </si>
@@ -663,12 +663,28 @@
 Data.value[0][2] = -1.3
 index = 0 </t>
   </si>
+  <si>
+    <t>aPartialNaNTest()</t>
+  </si>
+  <si>
+    <t>aFullyNaNTest()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Range = (-1.0,1.0)
+    b0 = null
+    b1 = 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Range = (-1.0,1.0)
+    b0 = null
+    b1 = null</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -700,6 +716,11 @@
       <color indexed="8"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -921,7 +942,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1016,6 +1037,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2179,8 +2203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1019"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -2977,12 +3001,22 @@
       <c r="Y22" s="5"/>
       <c r="Z22" s="5"/>
     </row>
-    <row r="23" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
+    <row r="23" spans="1:26" ht="46" customHeight="1">
+      <c r="A23" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="B23" s="33" t="s">
+        <v>164</v>
+      </c>
+      <c r="C23" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="D23" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>10</v>
+      </c>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
@@ -3005,12 +3039,22 @@
       <c r="Y23" s="5"/>
       <c r="Z23" s="5"/>
     </row>
-    <row r="24" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
+    <row r="24" spans="1:26" ht="46" customHeight="1">
+      <c r="A24" s="33" t="s">
+        <v>163</v>
+      </c>
+      <c r="B24" s="33" t="s">
+        <v>165</v>
+      </c>
+      <c r="C24" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>10</v>
+      </c>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
@@ -31466,6 +31510,7 @@
       <c r="Z1019" s="5"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <headerFooter>

</xml_diff>